<commit_message>
mod de excel para separaro los obojtos en directorios
</commit_message>
<xml_diff>
--- a/Diccionarios Datos/Detallado de Tablas.xlsx
+++ b/Diccionarios Datos/Detallado de Tablas.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja3!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja3!$D$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="194">
   <si>
     <t>BD</t>
   </si>
@@ -606,13 +606,16 @@
   </si>
   <si>
     <t>Accion</t>
+  </si>
+  <si>
+    <t>Esquema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,13 +632,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -643,7 +647,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -663,6 +666,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -767,86 +777,86 @@
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,2413 +1171,2492 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P74"/>
+  <dimension ref="D1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="11"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="35.5703125" customWidth="1"/>
+    <col min="1" max="3" width="11.42578125" style="32"/>
+    <col min="4" max="5" width="11.42578125" style="31"/>
+    <col min="6" max="6" width="15.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="32" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="32"/>
+    <col min="11" max="11" width="8.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="32" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="23" style="32" customWidth="1"/>
+    <col min="16" max="16" width="35.5703125" style="32" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="4:16" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="F1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="H1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="M1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="N1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="O1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="P1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="G2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="24">
+      <c r="H2" s="6">
         <v>2</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="K2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="L2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="M2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="15" t="s">
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="G3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="24">
+      <c r="H3" s="6">
         <v>5</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="I3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="J3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="K3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="13">
+      <c r="H4" s="13">
         <v>8</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="I4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="J4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="K4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="13">
+      <c r="H5" s="13">
         <v>11</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="I5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="J5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="K5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="13">
+      <c r="H6" s="13">
         <v>14</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="I6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="J6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="K6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="13">
+      <c r="H7" s="13">
         <v>17</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="I7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="J7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="K7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="G8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="27">
+      <c r="H8" s="15">
         <v>22</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="I8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="J8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="K8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="L8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="M8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20" t="s">
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="G9" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="19">
+      <c r="H9" s="17">
         <v>25</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="I9" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="J9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="K9" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="E10" s="14"/>
+      <c r="F10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="G10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="19">
+      <c r="H10" s="17">
         <v>28</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="I10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="J10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="K10" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="L10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="22" t="s">
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="E11" s="14"/>
+      <c r="F11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="G11" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="19">
+      <c r="H11" s="17">
         <v>31</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="I11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="J11" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="K11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="22" t="s">
+      <c r="L11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="E12" s="14"/>
+      <c r="F12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="G12" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="19">
+      <c r="H12" s="17">
         <v>34</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="I12" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="J12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="K12" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="G13" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="19">
+      <c r="H13" s="17">
         <v>37</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="I13" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="J13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="K13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="22" t="s">
+      <c r="L13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="E14" s="5"/>
+      <c r="F14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="G14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="24">
+      <c r="H14" s="6">
         <v>41</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="I14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="J14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="K14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="L14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="M14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="15" t="s">
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="G15" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="13">
+      <c r="H15" s="13">
         <v>44</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="I15" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="J15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="K15" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="G16" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="13">
+      <c r="H16" s="13">
         <v>47</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="I16" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="J16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="K16" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="E17" s="5"/>
+      <c r="F17" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="G17" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="13">
+      <c r="H17" s="13">
         <v>50</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="I17" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="J17" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="K17" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="E18" s="5"/>
+      <c r="F18" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="G18" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="13">
+      <c r="H18" s="13">
         <v>53</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="I18" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="J18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="K18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="L18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="15" t="s">
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="E19" s="14"/>
+      <c r="F19" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="G19" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="27">
+      <c r="H19" s="15">
         <v>57</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="I19" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="J19" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="28" t="s">
+      <c r="K19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="L19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="M19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="20" t="s">
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="E20" s="14"/>
+      <c r="F20" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="G20" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="27">
+      <c r="H20" s="15">
         <v>60</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="I20" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="J20" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="K20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="L20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="20" t="s">
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="E21" s="14"/>
+      <c r="F21" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="G21" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="19">
+      <c r="H21" s="17">
         <v>63</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="I21" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="J21" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="K21" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="H21" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="22" t="s">
+      <c r="L21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+    <row r="22" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="E22" s="14"/>
+      <c r="F22" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="G22" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="19">
+      <c r="H22" s="17">
         <v>66</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="I22" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="J22" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="K22" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="L22" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="20" t="s">
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="E23" s="14"/>
+      <c r="F23" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="G23" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="19">
+      <c r="H23" s="17">
         <v>69</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="I23" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="J23" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="K23" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="L23" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="20" t="s">
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="E24" s="14"/>
+      <c r="F24" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="G24" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="19">
+      <c r="H24" s="17">
         <v>72</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="I24" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="J24" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="K24" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="L24" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="20" t="s">
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="E25" s="14"/>
+      <c r="F25" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="G25" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="19">
+      <c r="H25" s="17">
         <v>75</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="I25" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="J25" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="K25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="L25" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="20" t="s">
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="E26" s="5"/>
+      <c r="F26" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="G26" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="24">
+      <c r="H26" s="6">
         <v>79</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="I26" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="J26" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="K26" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="L26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="24" t="s">
+      <c r="M26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="4" t="s">
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="E27" s="5"/>
+      <c r="F27" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="G27" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="24">
+      <c r="H27" s="6">
         <v>82</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="I27" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="J27" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="K27" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="25" t="s">
+      <c r="L27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="4" t="s">
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="E28" s="5"/>
+      <c r="F28" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="G28" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="13">
+      <c r="H28" s="13">
         <v>85</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="I28" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="J28" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="K28" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="4" t="s">
+      <c r="L28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="22" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="E29" s="5"/>
+      <c r="F29" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="G29" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="13">
+      <c r="H29" s="13">
         <v>88</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="I29" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="J29" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="K29" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="L29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="30"/>
-    </row>
-    <row r="30" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="28"/>
+    </row>
+    <row r="30" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="E30" s="5"/>
+      <c r="F30" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="G30" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="13">
+      <c r="H30" s="13">
         <v>91</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="I30" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="J30" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="K30" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="L30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="4" t="s">
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="22" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="E31" s="5"/>
+      <c r="F31" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="G31" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="13">
+      <c r="H31" s="13">
         <v>94</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="I31" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="J31" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="K31" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="L31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="4" t="s">
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="22" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="E32" s="5"/>
+      <c r="F32" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="G32" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="13">
+      <c r="H32" s="13">
         <v>97</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="I32" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="J32" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="K32" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="L32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="4" t="s">
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+    <row r="33" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="E33" s="14"/>
+      <c r="F33" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="G33" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="27">
+      <c r="H33" s="15">
         <v>101</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="I33" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="28" t="s">
+      <c r="J33" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="28" t="s">
+      <c r="K33" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="28" t="s">
+      <c r="L33" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I33" s="27" t="s">
+      <c r="M33" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="20" t="s">
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+    <row r="34" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="E34" s="14"/>
+      <c r="F34" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="G34" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="19">
+      <c r="H34" s="17">
         <v>104</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="I34" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="J34" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="K34" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="20" t="s">
+      <c r="L34" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+    <row r="35" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="E35" s="14"/>
+      <c r="F35" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="G35" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="19">
+      <c r="H35" s="17">
         <v>107</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="I35" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="J35" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="K35" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="L35" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="22" t="s">
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+    <row r="36" spans="4:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="E36" s="5"/>
+      <c r="F36" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="G36" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="24">
+      <c r="H36" s="6">
         <v>111</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="I36" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="J36" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="K36" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H36" s="24" t="s">
+      <c r="L36" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="24" t="s">
+      <c r="M36" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="13" t="s">
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-    </row>
-    <row r="37" spans="1:16" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+    </row>
+    <row r="37" spans="4:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="E37" s="5"/>
+      <c r="F37" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="G37" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="13">
+      <c r="H37" s="13">
         <v>114</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="I37" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="J37" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="K37" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
       <c r="L37" s="13" t="s">
-        <v>177</v>
+        <v>15</v>
       </c>
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
       <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-    </row>
-    <row r="38" spans="1:16" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="P37" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+    </row>
+    <row r="38" spans="4:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="E38" s="5"/>
+      <c r="F38" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="G38" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="13">
+      <c r="H38" s="13">
         <v>117</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="I38" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="J38" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="K38" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="L38" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13" t="s">
-        <v>178</v>
       </c>
       <c r="M38" s="13"/>
       <c r="N38" s="13"/>
       <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-    </row>
-    <row r="39" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="P38" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+    </row>
+    <row r="39" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="E39" s="14"/>
+      <c r="F39" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="G39" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="27">
+      <c r="H39" s="15">
         <v>121</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="I39" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="F39" s="28" t="s">
+      <c r="J39" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="28" t="s">
+      <c r="K39" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="28" t="s">
+      <c r="L39" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I39" s="27" t="s">
+      <c r="M39" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="20" t="s">
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+    <row r="40" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="E40" s="14"/>
+      <c r="F40" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="G40" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="27">
+      <c r="H40" s="15">
         <v>124</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="I40" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="F40" s="28" t="s">
+      <c r="J40" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="G40" s="29" t="s">
+      <c r="K40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="20" t="s">
+      <c r="L40" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+    <row r="41" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="E41" s="14"/>
+      <c r="F41" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="G41" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D41" s="27">
+      <c r="H41" s="15">
         <v>128</v>
       </c>
-      <c r="E41" s="29" t="s">
+      <c r="I41" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="F41" s="28" t="s">
+      <c r="J41" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="G41" s="29" t="s">
+      <c r="K41" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H41" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="22"/>
-    </row>
-    <row r="42" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
+      <c r="L41" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="20"/>
+    </row>
+    <row r="42" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="E42" s="14"/>
+      <c r="F42" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="G42" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D42" s="19">
+      <c r="H42" s="17">
         <v>130</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="I42" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="J42" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="22" t="s">
+      <c r="K42" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H42" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="22" t="s">
+      <c r="L42" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
+    <row r="43" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="E43" s="14"/>
+      <c r="F43" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="G43" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="19">
+      <c r="H43" s="17">
         <v>134</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="I43" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="J43" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="G43" s="22" t="s">
+      <c r="K43" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H43" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="22"/>
-    </row>
-    <row r="44" spans="1:16" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+      <c r="L43" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="20"/>
+    </row>
+    <row r="44" spans="4:20" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="E44" s="14"/>
+      <c r="F44" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="G44" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="19">
+      <c r="H44" s="17">
         <v>136</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="I44" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="J44" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="K44" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H44" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="22" t="s">
+      <c r="L44" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
+    <row r="45" spans="4:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="E45" s="5"/>
+      <c r="F45" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="G45" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="24">
+      <c r="H45" s="6">
         <v>140</v>
       </c>
-      <c r="E45" s="25" t="s">
+      <c r="I45" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F45" s="25" t="s">
+      <c r="J45" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G45" s="25" t="s">
+      <c r="K45" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="25" t="s">
+      <c r="L45" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I45" s="24" t="s">
+      <c r="M45" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="15" t="s">
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+    <row r="46" spans="4:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="E46" s="5"/>
+      <c r="F46" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="G46" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="13">
+      <c r="H46" s="13">
         <v>143</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="I46" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="J46" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="G46" s="17" t="s">
+      <c r="K46" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="H46" s="15" t="s">
+      <c r="L46" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="15" t="s">
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
+    <row r="47" spans="4:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="E47" s="5"/>
+      <c r="F47" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="G47" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D47" s="13">
+      <c r="H47" s="13">
         <v>146</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="I47" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="J47" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="K47" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H47" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="15" t="s">
+      <c r="L47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+    <row r="48" spans="4:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="E48" s="5"/>
+      <c r="F48" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="G48" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="13">
+      <c r="H48" s="13">
         <v>149</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="I48" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="J48" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="K48" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H48" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="17" t="s">
+      <c r="L48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+    <row r="49" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="E49" s="5"/>
+      <c r="F49" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="G49" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="13">
+      <c r="H49" s="13">
         <v>152</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="I49" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="J49" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G49" s="17" t="s">
+      <c r="K49" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="17" t="s">
+      <c r="L49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
+    <row r="50" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="E50" s="5"/>
+      <c r="F50" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="G50" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="13">
+      <c r="H50" s="13">
         <v>155</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="I50" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="J50" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G50" s="17" t="s">
+      <c r="K50" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H50" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="17" t="s">
+      <c r="L50" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
+    <row r="51" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="E51" s="5"/>
+      <c r="F51" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="G51" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="13">
+      <c r="H51" s="13">
         <v>158</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="I51" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="J51" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="17" t="s">
+      <c r="K51" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H51" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="17" t="s">
+      <c r="L51" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+    <row r="52" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="E52" s="5"/>
+      <c r="F52" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="G52" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D52" s="13">
+      <c r="H52" s="13">
         <v>161</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="I52" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="J52" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G52" s="17" t="s">
+      <c r="K52" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H52" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="17" t="s">
+      <c r="L52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+    <row r="53" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="E53" s="14"/>
+      <c r="F53" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="27" t="s">
+      <c r="G53" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="D53" s="27">
+      <c r="H53" s="15">
         <v>164</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="I53" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="F53" s="28" t="s">
+      <c r="J53" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="G53" s="29" t="s">
+      <c r="K53" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="H53" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I53" s="27" t="s">
+      <c r="L53" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M53" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
-      <c r="L53" s="23"/>
-    </row>
-    <row r="54" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="30"/>
+    </row>
+    <row r="54" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="E54" s="14"/>
+      <c r="F54" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="G54" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="D54" s="19">
+      <c r="H54" s="17">
         <v>167</v>
       </c>
-      <c r="E54" s="22" t="s">
+      <c r="I54" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F54" s="20" t="s">
+      <c r="J54" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="G54" s="22" t="s">
+      <c r="K54" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="H54" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I54" s="19"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
-      <c r="L54" s="23"/>
-    </row>
-    <row r="55" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="31" t="s">
+      <c r="L54" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="30"/>
+    </row>
+    <row r="55" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="E55" s="14"/>
+      <c r="F55" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="G55" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="D55" s="19">
+      <c r="H55" s="17">
         <v>170</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="I55" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="F55" s="20" t="s">
+      <c r="J55" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="G55" s="22" t="s">
+      <c r="K55" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="H55" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="23"/>
-    </row>
-    <row r="56" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="L55" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="30"/>
+    </row>
+    <row r="56" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="E56" s="14"/>
+      <c r="F56" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="G56" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="D56" s="19">
+      <c r="H56" s="17">
         <v>173</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="I56" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F56" s="20" t="s">
+      <c r="J56" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G56" s="22" t="s">
+      <c r="K56" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H56" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="23"/>
-    </row>
-    <row r="57" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+      <c r="L56" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="30"/>
+    </row>
+    <row r="57" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="E57" s="14"/>
+      <c r="F57" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="G57" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="D57" s="19">
+      <c r="H57" s="17">
         <v>175</v>
       </c>
-      <c r="E57" s="22" t="s">
+      <c r="I57" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F57" s="20" t="s">
+      <c r="J57" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G57" s="22" t="s">
+      <c r="K57" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H57" s="20" t="s">
+      <c r="L57" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="23"/>
-    </row>
-    <row r="58" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="30"/>
+    </row>
+    <row r="58" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D58" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="E58" s="5"/>
+      <c r="F58" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="G58" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D58" s="24">
+      <c r="H58" s="6">
         <v>178</v>
       </c>
-      <c r="E58" s="25" t="s">
+      <c r="I58" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="F58" s="25" t="s">
+      <c r="J58" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="G58" s="25" t="s">
+      <c r="K58" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="H58" s="25" t="s">
+      <c r="L58" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I58" s="24" t="s">
+      <c r="M58" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J58" s="24"/>
-      <c r="K58" s="24"/>
-      <c r="L58" s="15" t="s">
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
+    <row r="59" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="E59" s="5"/>
+      <c r="F59" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="G59" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D59" s="13">
+      <c r="H59" s="13">
         <v>181</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="I59" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F59" s="15" t="s">
+      <c r="J59" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G59" s="17" t="s">
+      <c r="K59" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H59" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="17" t="s">
+      <c r="L59" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+      <c r="P59" s="12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14" t="s">
+    <row r="60" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="E60" s="5"/>
+      <c r="F60" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="G60" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D60" s="13">
+      <c r="H60" s="13">
         <v>184</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="I60" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="F60" s="15" t="s">
+      <c r="J60" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="G60" s="17" t="s">
+      <c r="K60" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H60" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
-      <c r="K60" s="13"/>
-      <c r="L60" s="17" t="s">
+      <c r="L60" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+      <c r="P60" s="12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
+    <row r="61" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="E61" s="5"/>
+      <c r="F61" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="G61" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="13">
+      <c r="H61" s="13">
         <v>187</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="I61" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="F61" s="15" t="s">
+      <c r="J61" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="G61" s="17" t="s">
+      <c r="K61" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="H61" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
-      <c r="L61" s="17" t="s">
+      <c r="L61" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13"/>
+      <c r="P61" s="12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
+    <row r="62" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="E62" s="5"/>
+      <c r="F62" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="G62" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D62" s="13">
+      <c r="H62" s="13">
         <v>189</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="I62" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="F62" s="15" t="s">
+      <c r="J62" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G62" s="17" t="s">
+      <c r="K62" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H62" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="17" t="s">
+      <c r="L62" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M62" s="13"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+      <c r="P62" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14" t="s">
+    <row r="63" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="E63" s="5"/>
+      <c r="F63" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="G63" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="13">
+      <c r="H63" s="13">
         <v>192</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="I63" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F63" s="15" t="s">
+      <c r="J63" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G63" s="17" t="s">
+      <c r="K63" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H63" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="17" t="s">
+      <c r="L63" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M63" s="13"/>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13"/>
+      <c r="P63" s="12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
+    <row r="64" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B64" s="27" t="s">
+      <c r="E64" s="14"/>
+      <c r="F64" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="27" t="s">
+      <c r="G64" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D64" s="27">
+      <c r="H64" s="15">
         <v>196</v>
       </c>
-      <c r="E64" s="27" t="s">
+      <c r="I64" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="F64" s="27" t="s">
+      <c r="J64" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="G64" s="27" t="s">
+      <c r="K64" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H64" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I64" s="27" t="s">
+      <c r="L64" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="M64" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J64" s="27"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="20"/>
-    </row>
-    <row r="65" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="18" t="s">
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="18"/>
+    </row>
+    <row r="65" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="E65" s="14"/>
+      <c r="F65" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="G65" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D65" s="19">
+      <c r="H65" s="17">
         <v>199</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="I65" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="F65" s="19" t="s">
+      <c r="J65" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="K65" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="H65" s="19" t="s">
+      <c r="L65" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="22"/>
-    </row>
-    <row r="66" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="20"/>
+    </row>
+    <row r="66" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D66" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="E66" s="14"/>
+      <c r="F66" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="G66" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D66" s="19">
+      <c r="H66" s="17">
         <v>202</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="I66" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="F66" s="19" t="s">
+      <c r="J66" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="G66" s="19" t="s">
+      <c r="K66" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="H66" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="22"/>
-    </row>
-    <row r="67" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="18" t="s">
+      <c r="L66" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="20"/>
+    </row>
+    <row r="67" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B67" s="19" t="s">
+      <c r="E67" s="14"/>
+      <c r="F67" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="G67" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D67" s="19">
+      <c r="H67" s="17">
         <v>205</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="I67" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="F67" s="19" t="s">
+      <c r="J67" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G67" s="19" t="s">
+      <c r="K67" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H67" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
-      <c r="K67" s="19"/>
-      <c r="L67" s="22"/>
-    </row>
-    <row r="68" spans="1:12" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="L67" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="20"/>
+    </row>
+    <row r="68" spans="4:16" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="E68" s="14"/>
+      <c r="F68" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="G68" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D68" s="19">
+      <c r="H68" s="17">
         <v>207</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="I68" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="F68" s="19" t="s">
+      <c r="J68" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G68" s="19" t="s">
+      <c r="K68" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H68" s="19" t="s">
+      <c r="L68" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
-      <c r="K68" s="19"/>
-      <c r="L68" s="22"/>
-    </row>
-    <row r="69" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
+      <c r="P68" s="20"/>
+    </row>
+    <row r="69" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B69" s="24" t="s">
+      <c r="E69" s="5"/>
+      <c r="F69" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C69" s="24" t="s">
+      <c r="G69" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D69" s="24">
+      <c r="H69" s="6">
         <v>214</v>
       </c>
-      <c r="E69" s="25" t="s">
+      <c r="I69" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F69" s="25" t="s">
+      <c r="J69" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="G69" s="25" t="s">
+      <c r="K69" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="H69" s="25" t="s">
+      <c r="L69" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I69" s="24" t="s">
+      <c r="M69" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J69" s="24"/>
-      <c r="K69" s="24"/>
-      <c r="L69" s="15" t="s">
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
+    <row r="70" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D70" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="E70" s="5"/>
+      <c r="F70" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="G70" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D70" s="13">
+      <c r="H70" s="13">
         <v>217</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="I70" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="F70" s="15" t="s">
+      <c r="J70" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G70" s="17" t="s">
+      <c r="K70" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H70" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="17" t="s">
+      <c r="L70" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13"/>
+      <c r="O70" s="13"/>
+      <c r="P70" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
+    <row r="71" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D71" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="E71" s="5"/>
+      <c r="F71" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="G71" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D71" s="13">
+      <c r="H71" s="13">
         <v>221</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="I71" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="F71" s="15" t="s">
+      <c r="J71" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G71" s="17" t="s">
+      <c r="K71" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H71" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="17" t="s">
+      <c r="L71" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
+    <row r="72" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D72" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="E72" s="5"/>
+      <c r="F72" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="G72" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D72" s="13">
+      <c r="H72" s="13">
         <v>224</v>
       </c>
-      <c r="E72" s="17" t="s">
+      <c r="I72" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="F72" s="15" t="s">
+      <c r="J72" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="G72" s="17" t="s">
+      <c r="K72" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="H72" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
-      <c r="L72" s="17" t="s">
+      <c r="L72" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M72" s="13"/>
+      <c r="N72" s="13"/>
+      <c r="O72" s="13"/>
+      <c r="P72" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
+    <row r="73" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D73" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="E73" s="5"/>
+      <c r="F73" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="G73" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D73" s="13">
+      <c r="H73" s="13">
         <v>227</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="I73" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F73" s="15" t="s">
+      <c r="J73" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G73" s="17" t="s">
+      <c r="K73" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H73" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="17" t="s">
+      <c r="L73" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="74" spans="1:12" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="s">
+    <row r="74" spans="4:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D74" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="E74" s="5"/>
+      <c r="F74" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="G74" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D74" s="13">
+      <c r="H74" s="13">
         <v>230</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="I74" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="J74" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G74" s="17" t="s">
+      <c r="K74" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H74" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="17" t="s">
+      <c r="L74" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13"/>
+      <c r="O74" s="13"/>
+      <c r="P74" s="12" t="s">
         <v>165</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="D1:P1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>